<commit_message>
packing up for the day
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb154/raw/Table7_by_waters.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb154/raw/Table7_by_waters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb154/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F542C1-D79A-0C47-B30D-AE107E58F012}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8BA6DE-596A-A74D-9CF4-14B332F6635A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29660" yWindow="460" windowWidth="17480" windowHeight="26520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30160" yWindow="640" windowWidth="17480" windowHeight="26380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Total pounds</t>
   </si>
@@ -106,12 +106,6 @@
     <t>Seabase white</t>
   </si>
   <si>
-    <t>Miwrfiwa  KasaLaaexM (ksmskl Sm&amp;  ~</t>
-  </si>
-  <si>
-    <t>fauafontn:</t>
-  </si>
-  <si>
     <t>Greeting, kelp</t>
   </si>
   <si>
@@ -272,6 +266,18 @@
   </si>
   <si>
     <t>Total check 2</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Crab, market</t>
+  </si>
+  <si>
+    <t>Miscellaneous (animal food)</t>
+  </si>
+  <si>
+    <t>Total check</t>
   </si>
 </sst>
 </file>
@@ -328,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -338,6 +344,7 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,61 +659,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:K1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.83203125" style="5"/>
     <col min="12" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -738,7 +744,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2">
         <v>22508</v>
@@ -763,7 +769,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2">
         <v>412430</v>
@@ -785,7 +791,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2">
         <v>1186419</v>
@@ -970,7 +976,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2">
         <v>146</v>
@@ -992,7 +998,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2">
         <v>7142</v>
@@ -1108,7 +1114,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2">
         <v>1508252</v>
@@ -1327,7 +1333,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B29" s="2">
         <v>6610661</v>
@@ -1446,7 +1452,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2">
         <v>76313</v>
@@ -1521,7 +1527,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" s="2">
         <v>386597</v>
@@ -1546,191 +1552,301 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="B39" s="2">
+        <v>3517</v>
+      </c>
+      <c r="D39" s="2">
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="C43" s="2">
+        <v>1232452</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="C44" s="2">
+        <v>44952</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="C45" s="2">
+        <v>71434</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
+      </c>
+      <c r="C46" s="2">
+        <v>72715</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="C47" s="2">
+        <v>362</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="D49" s="2">
+        <v>16633</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="C50" s="2">
+        <v>1474172</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2511435</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="D51" s="4">
+        <v>18325</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G58" s="4"/>
       <c r="H58" s="6"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>29</v>
+        <v>84</v>
+      </c>
+      <c r="C60" s="2">
+        <v>77234</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+      <c r="C68" s="2">
+        <v>95765</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1" t="s">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" s="2">
+        <v>373374212</v>
+      </c>
+      <c r="C76" s="2">
+        <v>3455304</v>
+      </c>
+      <c r="D76" s="2">
+        <v>309239014</v>
+      </c>
+      <c r="E76" s="2">
+        <v>4231225</v>
+      </c>
+      <c r="F76" s="2">
+        <v>6835749</v>
+      </c>
+      <c r="G76" s="2">
+        <v>703215505</v>
+      </c>
+      <c r="H76" s="1"/>
+      <c r="I76" s="5">
+        <v>95189616</v>
+      </c>
+      <c r="J76" s="2">
+        <v>739415322</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" s="5">
+        <f>B76-SUM(B2:B75)</f>
+        <v>94787761</v>
+      </c>
+      <c r="C77" s="5">
+        <f t="shared" ref="C77:J77" si="2">C76-SUM(C2:C75)</f>
+        <v>-9759</v>
+      </c>
+      <c r="D77" s="5">
+        <f t="shared" si="2"/>
+        <v>305328918</v>
+      </c>
+      <c r="E77" s="5">
+        <f t="shared" si="2"/>
+        <v>4231225</v>
+      </c>
+      <c r="F77" s="5">
+        <f t="shared" si="2"/>
+        <v>6835749</v>
+      </c>
+      <c r="G77" s="5">
+        <f t="shared" si="2"/>
+        <v>422873154</v>
+      </c>
+      <c r="H77" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I77" s="5">
+        <f t="shared" si="2"/>
+        <v>95189616</v>
+      </c>
+      <c r="J77" s="5">
+        <f t="shared" si="2"/>
+        <v>459072971</v>
+      </c>
+      <c r="K77" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>